<commit_message>
updated docs for pages
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-glstring-codesystem.xlsx
+++ b/docs/CodeSystem-glstring-codesystem.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Property</t>
   </si>
@@ -53,10 +53,13 @@
     <t>Experimental</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2023-01-12T09:36:27-06:00</t>
+    <t>2023-02-16T14:43:10-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -96,9 +99,6 @@
   </si>
   <si>
     <t>Compositional</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>Version Needed?</t>
@@ -309,78 +309,82 @@
       <c r="A7" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">

</xml_diff>